<commit_message>
Terminando epigrafe Datos delcapitulo 2
</commit_message>
<xml_diff>
--- a/data/000_empresas.xlsx
+++ b/data/000_empresas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\APPs\TFM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{530B5512-1286-42A4-BC73-661BAADBE22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A79C9C-A5D5-4177-A5BC-842D907DA9E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="345" windowWidth="15180" windowHeight="9840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="277">
   <si>
     <t>ACCIONA,S.A.</t>
   </si>
@@ -441,9 +441,6 @@
     <t>SACYR, S.A.</t>
   </si>
   <si>
-    <t>SIEMENS GAMESA RENEWABLE ENERGY, S.A.</t>
-  </si>
-  <si>
     <t>SOLARIA ENERGIA Y MEDIO AMBIENTE, S.A.</t>
   </si>
   <si>
@@ -669,9 +666,6 @@
     <t>FCC.MC</t>
   </si>
   <si>
-    <t>GALQ.MC</t>
-  </si>
-  <si>
     <t>GEST.MC</t>
   </si>
   <si>
@@ -822,9 +816,6 @@
     <t>SCYR.MC</t>
   </si>
   <si>
-    <t>SGRE.MC</t>
-  </si>
-  <si>
     <t>SLR.MC</t>
   </si>
   <si>
@@ -862,6 +853,9 @@
   </si>
   <si>
     <t>VOC.MC</t>
+  </si>
+  <si>
+    <t>GAM.MC</t>
   </si>
 </sst>
 </file>
@@ -1236,10 +1230,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F123"/>
+  <dimension ref="B2:F122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="B96" workbookViewId="0">
+      <selection activeCell="B110" sqref="A110:XFD110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1253,19 +1247,19 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>154</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -1273,7 +1267,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>1</v>
@@ -1290,7 +1284,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>5</v>
@@ -1307,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>1</v>
@@ -1324,7 +1318,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>9</v>
@@ -1341,7 +1335,7 @@
         <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>12</v>
@@ -1358,7 +1352,7 @@
         <v>13</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>14</v>
@@ -1375,7 +1369,7 @@
         <v>15</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>16</v>
@@ -1392,7 +1386,7 @@
         <v>17</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>18</v>
@@ -1409,7 +1403,7 @@
         <v>19</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>20</v>
@@ -1426,7 +1420,7 @@
         <v>21</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>22</v>
@@ -1443,7 +1437,7 @@
         <v>23</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>24</v>
@@ -1460,7 +1454,7 @@
         <v>25</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>24</v>
@@ -1477,7 +1471,7 @@
         <v>26</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>27</v>
@@ -1494,7 +1488,7 @@
         <v>28</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>5</v>
@@ -1509,7 +1503,7 @@
         <v>29</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>18</v>
@@ -1526,7 +1520,7 @@
         <v>30</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>5</v>
@@ -1543,7 +1537,7 @@
         <v>31</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>32</v>
@@ -1560,7 +1554,7 @@
         <v>33</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>34</v>
@@ -1577,7 +1571,7 @@
         <v>35</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>22</v>
@@ -1594,7 +1588,7 @@
         <v>36</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>37</v>
@@ -1611,7 +1605,7 @@
         <v>38</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>39</v>
@@ -1628,7 +1622,7 @@
         <v>40</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>41</v>
@@ -1645,7 +1639,7 @@
         <v>42</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>41</v>
@@ -1662,7 +1656,7 @@
         <v>43</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>41</v>
@@ -1679,7 +1673,7 @@
         <v>44</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>41</v>
@@ -1696,7 +1690,7 @@
         <v>45</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>5</v>
@@ -1713,7 +1707,7 @@
         <v>46</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>47</v>
@@ -1730,7 +1724,7 @@
         <v>48</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>47</v>
@@ -1745,7 +1739,7 @@
         <v>49</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>41</v>
@@ -1762,7 +1756,7 @@
         <v>50</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>41</v>
@@ -1777,7 +1771,7 @@
         <v>51</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>52</v>
@@ -1794,7 +1788,7 @@
         <v>54</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>55</v>
@@ -1811,7 +1805,7 @@
         <v>56</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>14</v>
@@ -1828,7 +1822,7 @@
         <v>57</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>12</v>
@@ -1843,7 +1837,7 @@
         <v>58</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>1</v>
@@ -1858,7 +1852,7 @@
         <v>59</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>5</v>
@@ -1875,7 +1869,7 @@
         <v>60</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>52</v>
@@ -1892,7 +1886,7 @@
         <v>61</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>47</v>
@@ -1909,7 +1903,7 @@
         <v>62</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>39</v>
@@ -1926,7 +1920,7 @@
         <v>63</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>37</v>
@@ -1943,7 +1937,7 @@
         <v>64</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>20</v>
@@ -1960,7 +1954,7 @@
         <v>65</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>47</v>
@@ -1977,7 +1971,7 @@
         <v>66</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>5</v>
@@ -1992,7 +1986,7 @@
         <v>67</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>68</v>
@@ -2009,7 +2003,7 @@
         <v>69</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>18</v>
@@ -2026,7 +2020,7 @@
         <v>70</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>47</v>
@@ -2043,7 +2037,7 @@
         <v>71</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>27</v>
@@ -2060,7 +2054,7 @@
         <v>72</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>39</v>
@@ -2077,7 +2071,7 @@
         <v>73</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>74</v>
@@ -2094,7 +2088,7 @@
         <v>75</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D52" s="5" t="s">
         <v>76</v>
@@ -2111,7 +2105,7 @@
         <v>77</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>74</v>
@@ -2128,7 +2122,7 @@
         <v>78</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>79</v>
@@ -2145,7 +2139,7 @@
         <v>80</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>22</v>
@@ -2162,7 +2156,7 @@
         <v>81</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>1</v>
@@ -2179,7 +2173,7 @@
         <v>82</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D57" s="6" t="s">
         <v>18</v>
@@ -2196,7 +2190,7 @@
         <v>83</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D58" s="6" t="s">
         <v>1</v>
@@ -2213,7 +2207,7 @@
         <v>84</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>214</v>
+        <v>276</v>
       </c>
       <c r="D59" s="6" t="s">
         <v>18</v>
@@ -2225,12 +2219,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="2:6" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D60" s="6" t="s">
         <v>39</v>
@@ -2247,7 +2241,7 @@
         <v>86</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>55</v>
@@ -2264,7 +2258,7 @@
         <v>87</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>37</v>
@@ -2281,7 +2275,7 @@
         <v>88</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D63" s="6" t="s">
         <v>22</v>
@@ -2298,7 +2292,7 @@
         <v>89</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D64" s="6" t="s">
         <v>90</v>
@@ -2315,7 +2309,7 @@
         <v>91</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>37</v>
@@ -2332,7 +2326,7 @@
         <v>92</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D66" s="6" t="s">
         <v>1</v>
@@ -2349,7 +2343,7 @@
         <v>93</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D67" s="6" t="s">
         <v>55</v>
@@ -2364,7 +2358,7 @@
         <v>94</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D68" s="6" t="s">
         <v>74</v>
@@ -2381,7 +2375,7 @@
         <v>95</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D69" s="6" t="s">
         <v>76</v>
@@ -2398,7 +2392,7 @@
         <v>96</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D70" s="6" t="s">
         <v>24</v>
@@ -2415,7 +2409,7 @@
         <v>97</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D71" s="6" t="s">
         <v>9</v>
@@ -2432,7 +2426,7 @@
         <v>98</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D72" s="6" t="s">
         <v>32</v>
@@ -2449,7 +2443,7 @@
         <v>99</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>12</v>
@@ -2466,7 +2460,7 @@
         <v>100</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D74" s="6" t="s">
         <v>68</v>
@@ -2481,7 +2475,7 @@
         <v>101</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D75" s="6" t="s">
         <v>14</v>
@@ -2498,7 +2492,7 @@
         <v>102</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D76" s="6" t="s">
         <v>22</v>
@@ -2515,7 +2509,7 @@
         <v>103</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D77" s="6" t="s">
         <v>22</v>
@@ -2532,7 +2526,7 @@
         <v>104</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D78" s="6" t="s">
         <v>32</v>
@@ -2549,7 +2543,7 @@
         <v>105</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D79" s="6" t="s">
         <v>12</v>
@@ -2564,7 +2558,7 @@
         <v>106</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D80" s="6" t="s">
         <v>90</v>
@@ -2581,7 +2575,7 @@
         <v>107</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D81" s="6" t="s">
         <v>5</v>
@@ -2596,7 +2590,7 @@
         <v>108</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D82" s="6" t="s">
         <v>90</v>
@@ -2613,7 +2607,7 @@
         <v>109</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D83" s="6" t="s">
         <v>34</v>
@@ -2630,7 +2624,7 @@
         <v>110</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D84" s="6" t="s">
         <v>27</v>
@@ -2647,7 +2641,7 @@
         <v>111</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D85" s="6" t="s">
         <v>32</v>
@@ -2664,7 +2658,7 @@
         <v>112</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D86" s="6" t="s">
         <v>12</v>
@@ -2681,7 +2675,7 @@
         <v>113</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D87" s="6" t="s">
         <v>76</v>
@@ -2698,7 +2692,7 @@
         <v>114</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D88" s="6" t="s">
         <v>12</v>
@@ -2713,7 +2707,7 @@
         <v>115</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D89" s="6" t="s">
         <v>74</v>
@@ -2730,7 +2724,7 @@
         <v>116</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D90" s="6" t="s">
         <v>47</v>
@@ -2747,7 +2741,7 @@
         <v>117</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D91" s="6" t="s">
         <v>12</v>
@@ -2764,7 +2758,7 @@
         <v>118</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D92" s="6" t="s">
         <v>27</v>
@@ -2781,7 +2775,7 @@
         <v>119</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D93" s="6" t="s">
         <v>39</v>
@@ -2798,7 +2792,7 @@
         <v>120</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D94" s="6" t="s">
         <v>9</v>
@@ -2815,7 +2809,7 @@
         <v>121</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D95" s="6" t="s">
         <v>12</v>
@@ -2832,7 +2826,7 @@
         <v>122</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D96" s="6" t="s">
         <v>1</v>
@@ -2849,7 +2843,7 @@
         <v>123</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D97" s="6" t="s">
         <v>37</v>
@@ -2866,7 +2860,7 @@
         <v>124</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D98" s="6" t="s">
         <v>22</v>
@@ -2883,7 +2877,7 @@
         <v>125</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D99" s="6" t="s">
         <v>47</v>
@@ -2900,7 +2894,7 @@
         <v>126</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D100" s="6" t="s">
         <v>22</v>
@@ -2917,7 +2911,7 @@
         <v>127</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D101" s="6" t="s">
         <v>22</v>
@@ -2934,7 +2928,7 @@
         <v>128</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D102" s="6" t="s">
         <v>34</v>
@@ -2951,7 +2945,7 @@
         <v>129</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D103" s="6" t="s">
         <v>52</v>
@@ -2968,7 +2962,7 @@
         <v>130</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D104" s="6" t="s">
         <v>12</v>
@@ -2985,7 +2979,7 @@
         <v>131</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D105" s="6" t="s">
         <v>74</v>
@@ -3002,7 +2996,7 @@
         <v>132</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D106" s="6" t="s">
         <v>133</v>
@@ -3019,7 +3013,7 @@
         <v>134</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D107" s="6" t="s">
         <v>12</v>
@@ -3036,7 +3030,7 @@
         <v>135</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D108" s="6" t="s">
         <v>136</v>
@@ -3053,7 +3047,7 @@
         <v>137</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D109" s="6" t="s">
         <v>1</v>
@@ -3065,27 +3059,29 @@
         <v>6</v>
       </c>
     </row>
-    <row r="110" spans="2:6" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B110" s="2" t="s">
         <v>138</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E110" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F110" s="6"/>
+      <c r="F110" s="6" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="111" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B111" s="2" t="s">
         <v>139</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D111" s="6" t="s">
         <v>37</v>
@@ -3094,7 +3090,7 @@
         <v>2</v>
       </c>
       <c r="F111" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="112" spans="2:6" x14ac:dyDescent="0.25">
@@ -3102,42 +3098,42 @@
         <v>140</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E112" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F112" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F112" s="6"/>
+    </row>
+    <row r="113" spans="2:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B113" s="2" t="s">
         <v>141</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D113" s="6" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E113" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F113" s="6"/>
-    </row>
-    <row r="114" spans="2:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F113" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="114" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B114" s="2" t="s">
         <v>142</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="E114" s="6" t="s">
         <v>2</v>
@@ -3146,38 +3142,38 @@
         <v>10</v>
       </c>
     </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B115" s="2" t="s">
         <v>143</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D115" s="6" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="E115" s="6" t="s">
         <v>2</v>
       </c>
       <c r="F115" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="116" spans="2:6" ht="25.5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="116" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B116" s="2" t="s">
         <v>144</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="E116" s="6" t="s">
         <v>2</v>
       </c>
       <c r="F116" s="6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="117" spans="2:6" x14ac:dyDescent="0.25">
@@ -3185,7 +3181,7 @@
         <v>145</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D117" s="6" t="s">
         <v>5</v>
@@ -3202,16 +3198,16 @@
         <v>146</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D118" s="6" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="E118" s="6" t="s">
         <v>2</v>
       </c>
       <c r="F118" s="6" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="119" spans="2:6" x14ac:dyDescent="0.25">
@@ -3219,16 +3215,16 @@
         <v>147</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D119" s="6" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="E119" s="6" t="s">
         <v>2</v>
       </c>
       <c r="F119" s="6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="120" spans="2:6" x14ac:dyDescent="0.25">
@@ -3236,10 +3232,10 @@
         <v>148</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>12</v>
+        <v>149</v>
       </c>
       <c r="E120" s="6" t="s">
         <v>2</v>
@@ -3250,19 +3246,19 @@
     </row>
     <row r="121" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B121" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D121" s="6" t="s">
-        <v>150</v>
+        <v>47</v>
       </c>
       <c r="E121" s="6" t="s">
         <v>2</v>
       </c>
       <c r="F121" s="6" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
     </row>
     <row r="122" spans="2:6" x14ac:dyDescent="0.25">
@@ -3270,32 +3266,15 @@
         <v>151</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="E122" s="6" t="s">
         <v>2</v>
       </c>
       <c r="F122" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B123" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C123" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="D123" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E123" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F123" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3408,23 +3387,22 @@
     <hyperlink ref="B107" r:id="rId105" display="https://www.bolsasymercados.es/bme-exchange/es/Mercados-y-Cotizaciones/Acciones/Mercado-Continuo/Ficha/Renta-Corporacion-Real-Estate-S-A-ES0173365018" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
     <hyperlink ref="B108" r:id="rId106" display="https://www.bolsasymercados.es/bme-exchange/es/Mercados-y-Cotizaciones/Acciones/Mercado-Continuo/Ficha/Repsol-S-A-ES0173516115" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
     <hyperlink ref="B109" r:id="rId107" display="https://www.bolsasymercados.es/bme-exchange/es/Mercados-y-Cotizaciones/Acciones/Mercado-Continuo/Ficha/Sacyr-S-A-ES0182870214" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
-    <hyperlink ref="B110" r:id="rId108" display="https://www.bolsasymercados.es/bme-exchange/es/Mercados-y-Cotizaciones/Acciones/Mercado-Continuo/Ficha/Siemens-Gamesa-Renewable-Energy-S-A-ES0143416115" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="B111" r:id="rId109" display="https://www.bolsasymercados.es/bme-exchange/es/Mercados-y-Cotizaciones/Acciones/Mercado-Continuo/Ficha/Solaria-Energia-Y-Medio-Ambiente-S-A-ES0165386014" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
-    <hyperlink ref="B112" r:id="rId110" display="https://www.bolsasymercados.es/bme-exchange/es/Mercados-y-Cotizaciones/Acciones/Mercado-Continuo/Ficha/Soltec-Power-Holdings-S-A-ES0105513008" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="B113" r:id="rId111" display="https://www.bolsasymercados.es/bme-exchange/es/Mercados-y-Cotizaciones/Acciones/Mercado-Continuo/Ficha/Squirrel-Media-S-A-ES0183304080" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="B114" r:id="rId112" display="https://www.bolsasymercados.es/bme-exchange/es/Mercados-y-Cotizaciones/Acciones/Mercado-Continuo/Ficha/Talgo-S-A-ES0105065009" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="B115" r:id="rId113" display="https://www.bolsasymercados.es/bme-exchange/es/Mercados-y-Cotizaciones/Acciones/Mercado-Continuo/Ficha/Tecnicas-Reunidas-S-A-ES0178165017" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
-    <hyperlink ref="B116" r:id="rId114" display="https://www.bolsasymercados.es/bme-exchange/es/Mercados-y-Cotizaciones/Acciones/Mercado-Continuo/Ficha/Telefonica-S-A-ES0178430E18" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="B117" r:id="rId115" display="https://www.bolsasymercados.es/bme-exchange/es/Mercados-y-Cotizaciones/Acciones/Mercado-Continuo/Ficha/Tubacex-S-A-ES0132945017" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="B118" r:id="rId116" display="https://www.bolsasymercados.es/bme-exchange/es/Mercados-y-Cotizaciones/Acciones/Mercado-Continuo/Ficha/Tubos-Reunidos-S-A-ES0180850416" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="B119" r:id="rId117" display="https://www.bolsasymercados.es/bme-exchange/es/Mercados-y-Cotizaciones/Acciones/Mercado-Continuo/Ficha/Unicaja-Banco-S-A-ES0180907000" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
-    <hyperlink ref="B120" r:id="rId118" display="https://www.bolsasymercados.es/bme-exchange/es/Mercados-y-Cotizaciones/Acciones/Mercado-Continuo/Ficha/Urbas-Grupo-Financiero-S-A-ES0182280018" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
-    <hyperlink ref="B121" r:id="rId119" display="https://www.bolsasymercados.es/bme-exchange/es/Mercados-y-Cotizaciones/Acciones/Mercado-Continuo/Ficha/Vidrala-S-A-ES0183746314" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
-    <hyperlink ref="B122" r:id="rId120" display="https://www.bolsasymercados.es/bme-exchange/es/Mercados-y-Cotizaciones/Acciones/Mercado-Continuo/Ficha/Viscofan-S-A-ES0184262212" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
-    <hyperlink ref="B123" r:id="rId121" display="https://www.bolsasymercados.es/bme-exchange/es/Mercados-y-Cotizaciones/Acciones/Mercado-Continuo/Ficha/Vocento-S-A-ES0114820113" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
-    <hyperlink ref="C91" r:id="rId122" xr:uid="{4D73DAD5-53E2-4F1A-992F-4BCFEF24A03F}"/>
+    <hyperlink ref="B110" r:id="rId108" display="https://www.bolsasymercados.es/bme-exchange/es/Mercados-y-Cotizaciones/Acciones/Mercado-Continuo/Ficha/Solaria-Energia-Y-Medio-Ambiente-S-A-ES0165386014" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="B111" r:id="rId109" display="https://www.bolsasymercados.es/bme-exchange/es/Mercados-y-Cotizaciones/Acciones/Mercado-Continuo/Ficha/Soltec-Power-Holdings-S-A-ES0105513008" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="B112" r:id="rId110" display="https://www.bolsasymercados.es/bme-exchange/es/Mercados-y-Cotizaciones/Acciones/Mercado-Continuo/Ficha/Squirrel-Media-S-A-ES0183304080" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="B113" r:id="rId111" display="https://www.bolsasymercados.es/bme-exchange/es/Mercados-y-Cotizaciones/Acciones/Mercado-Continuo/Ficha/Talgo-S-A-ES0105065009" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="B114" r:id="rId112" display="https://www.bolsasymercados.es/bme-exchange/es/Mercados-y-Cotizaciones/Acciones/Mercado-Continuo/Ficha/Tecnicas-Reunidas-S-A-ES0178165017" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="B115" r:id="rId113" display="https://www.bolsasymercados.es/bme-exchange/es/Mercados-y-Cotizaciones/Acciones/Mercado-Continuo/Ficha/Telefonica-S-A-ES0178430E18" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="B116" r:id="rId114" display="https://www.bolsasymercados.es/bme-exchange/es/Mercados-y-Cotizaciones/Acciones/Mercado-Continuo/Ficha/Tubacex-S-A-ES0132945017" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="B117" r:id="rId115" display="https://www.bolsasymercados.es/bme-exchange/es/Mercados-y-Cotizaciones/Acciones/Mercado-Continuo/Ficha/Tubos-Reunidos-S-A-ES0180850416" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="B118" r:id="rId116" display="https://www.bolsasymercados.es/bme-exchange/es/Mercados-y-Cotizaciones/Acciones/Mercado-Continuo/Ficha/Unicaja-Banco-S-A-ES0180907000" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="B119" r:id="rId117" display="https://www.bolsasymercados.es/bme-exchange/es/Mercados-y-Cotizaciones/Acciones/Mercado-Continuo/Ficha/Urbas-Grupo-Financiero-S-A-ES0182280018" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="B120" r:id="rId118" display="https://www.bolsasymercados.es/bme-exchange/es/Mercados-y-Cotizaciones/Acciones/Mercado-Continuo/Ficha/Vidrala-S-A-ES0183746314" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="B121" r:id="rId119" display="https://www.bolsasymercados.es/bme-exchange/es/Mercados-y-Cotizaciones/Acciones/Mercado-Continuo/Ficha/Viscofan-S-A-ES0184262212" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="B122" r:id="rId120" display="https://www.bolsasymercados.es/bme-exchange/es/Mercados-y-Cotizaciones/Acciones/Mercado-Continuo/Ficha/Vocento-S-A-ES0114820113" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="C91" r:id="rId121" xr:uid="{4D73DAD5-53E2-4F1A-992F-4BCFEF24A03F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId123"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId122"/>
 </worksheet>
 </file>
</xml_diff>